<commit_message>
add new styles and functionality
</commit_message>
<xml_diff>
--- a/xlsx_files/Race63.xlsx
+++ b/xlsx_files/Race63.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Elo_new\xlsx_files_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F26DCF7-1C86-4218-A1EC-7F70A5BA5273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E614FE-5C56-4FEA-A715-AFC8393EA682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,7 +522,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>